<commit_message>
Der Zeitplan wurde aktualisiert
</commit_message>
<xml_diff>
--- a/TP/Dateien/Zeitplan.xlsx
+++ b/TP/Dateien/Zeitplan.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -18,6 +18,57 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>Planung</t>
+  </si>
+  <si>
+    <t>Prozessmodell definieren</t>
+  </si>
+  <si>
+    <t>Anforderungsspezifikation</t>
+  </si>
+  <si>
+    <t>Pflichtenheft</t>
+  </si>
+  <si>
+    <t>Find ideas</t>
+  </si>
+  <si>
+    <t>In the internet</t>
+  </si>
+  <si>
+    <t>In the real world</t>
+  </si>
+  <si>
+    <t>Programming</t>
+  </si>
+  <si>
+    <t>Defining the Content</t>
+  </si>
+  <si>
+    <t>Write content</t>
+  </si>
+  <si>
+    <t>Find content</t>
+  </si>
+  <si>
+    <t>CMS Webseite
+Industrie 4.0: Connectivity</t>
+  </si>
+  <si>
+    <t>Einarbeitung CMS</t>
+  </si>
+  <si>
+    <t>Content definieren</t>
+  </si>
+  <si>
+    <t>Zeitplan</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
@@ -29,15 +80,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -45,15 +114,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -331,12 +507,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1">
+        <v>60</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="16"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5">
+        <v>2</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="A1:A13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B1:B13"/>
+    <mergeCell ref="C1:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D1:D5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fehler in der Zeitberechnung wurden ausgebessert
</commit_message>
<xml_diff>
--- a/TP/Dateien/Zeitplan.xlsx
+++ b/TP/Dateien/Zeitplan.xlsx
@@ -200,6 +200,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -225,12 +231,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -516,7 +516,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,16 +527,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="10">
-        <v>60</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="12">
+        <v>36</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10">
+      <c r="D1" s="12">
         <v>20</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -547,10 +547,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="12"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -559,10 +559,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="12"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
@@ -571,32 +571,32 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="19" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="12">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="11"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="16" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="12">
         <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -607,10 +607,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="11"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
@@ -619,12 +619,12 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="16" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="12">
         <v>9</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -635,30 +635,30 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="19" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="12">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="11"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="11"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="8" t="s">
         <v>15</v>
       </c>
@@ -667,12 +667,12 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="16" t="s">
+      <c r="A12" s="16"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="12">
         <v>4</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -683,10 +683,10 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="11"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="3" t="s">
         <v>10</v>
       </c>
@@ -698,18 +698,18 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:A13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B1:B13"/>
+    <mergeCell ref="C1:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C11"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="D8:D11"/>
-    <mergeCell ref="A1:A13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B1:B13"/>
-    <mergeCell ref="C1:C5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C11"/>
     <mergeCell ref="D1:D5"/>
     <mergeCell ref="D6:D7"/>
   </mergeCells>

</xml_diff>